<commit_message>
revise figures for report
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJPF_Decrements_AV2020.xlsx
+++ b/inputs/data_raw/Data_SJPF_Decrements_AV2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C78E0-3070-494D-BABF-37E6120D9C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280AB17E-5607-418C-A53C-EF534D091BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="43" r:id="rId1"/>
@@ -904,6 +904,10 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -931,10 +935,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2160,18 +2160,18 @@
       <c r="N5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="73" t="s">
+      <c r="Q5" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="73"/>
-      <c r="S5" s="74" t="s">
+      <c r="R5" s="75"/>
+      <c r="S5" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="T5" s="74"/>
-      <c r="U5" s="75" t="s">
+      <c r="T5" s="76"/>
+      <c r="U5" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="75"/>
+      <c r="V5" s="77"/>
     </row>
     <row r="6" spans="1:22" ht="15.75">
       <c r="C6" s="25" t="s">
@@ -2953,20 +2953,20 @@
     <row r="5" spans="1:15" ht="15.75">
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
     </row>
     <row r="6" spans="1:15" ht="15.75">
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-    </row>
-    <row r="7" spans="1:15" ht="31.5">
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.75">
       <c r="D7" s="56" t="s">
         <v>49</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="N7" s="18"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="31.5">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="C7" s="46">
         <v>20</v>
       </c>
-      <c r="D7" s="78">
+      <c r="D7" s="69">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="E7" s="47"/>
@@ -4961,7 +4961,7 @@
       <c r="C8" s="46">
         <v>30</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="69">
         <v>1.67E-3</v>
       </c>
       <c r="E8" s="48"/>
@@ -4973,7 +4973,7 @@
       <c r="C9" s="46">
         <v>40</v>
       </c>
-      <c r="D9" s="78">
+      <c r="D9" s="69">
         <v>4.64E-3</v>
       </c>
       <c r="E9" s="48"/>
@@ -4985,7 +4985,7 @@
       <c r="C10" s="46">
         <v>50</v>
       </c>
-      <c r="D10" s="78">
+      <c r="D10" s="69">
         <v>1.027E-2</v>
       </c>
       <c r="E10" s="48"/>
@@ -4997,7 +4997,7 @@
       <c r="C11" s="46">
         <v>60</v>
       </c>
-      <c r="D11" s="78">
+      <c r="D11" s="69">
         <v>1.966E-2</v>
       </c>
       <c r="E11" s="48"/>
@@ -5009,7 +5009,7 @@
       <c r="C12" s="46">
         <v>70</v>
       </c>
-      <c r="D12" s="78">
+      <c r="D12" s="69">
         <v>3.4029999999999998E-2</v>
       </c>
       <c r="E12" s="48"/>
@@ -5021,7 +5021,7 @@
       <c r="C13" s="46">
         <v>80</v>
       </c>
-      <c r="D13" s="78">
+      <c r="D13" s="69">
         <v>5.4739999999999997E-2</v>
       </c>
       <c r="E13" s="48"/>
@@ -5033,7 +5033,7 @@
       <c r="C14" s="46">
         <v>20</v>
       </c>
-      <c r="D14" s="78">
+      <c r="D14" s="69">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
       <c r="C15" s="46">
         <v>30</v>
       </c>
-      <c r="D15" s="78">
+      <c r="D15" s="69">
         <v>5.5999999999999995E-4</v>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       <c r="C16" s="46">
         <v>40</v>
       </c>
-      <c r="D16" s="78">
+      <c r="D16" s="69">
         <v>2.2499999999999998E-3</v>
       </c>
     </row>
@@ -5066,7 +5066,7 @@
       <c r="C17" s="46">
         <v>50</v>
       </c>
-      <c r="D17" s="78">
+      <c r="D17" s="69">
         <v>2.0789999999999999E-2</v>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       <c r="C18" s="46">
         <v>60</v>
       </c>
-      <c r="D18" s="78">
+      <c r="D18" s="69">
         <v>4.3749999999999997E-2</v>
       </c>
     </row>
@@ -5088,7 +5088,7 @@
       <c r="C19" s="46">
         <v>70</v>
       </c>
-      <c r="D19" s="78">
+      <c r="D19" s="69">
         <v>8.2210000000000005E-2</v>
       </c>
     </row>
@@ -5099,7 +5099,7 @@
       <c r="C20" s="46">
         <v>80</v>
       </c>
-      <c r="D20" s="78">
+      <c r="D20" s="69">
         <v>0.14219000000000001</v>
       </c>
     </row>
@@ -5110,7 +5110,7 @@
       <c r="C21" s="46">
         <v>20</v>
       </c>
-      <c r="D21" s="78">
+      <c r="D21" s="69">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       <c r="C22" s="46">
         <v>30</v>
       </c>
-      <c r="D22" s="78">
+      <c r="D22" s="69">
         <v>5.5999999999999995E-4</v>
       </c>
     </row>
@@ -5132,7 +5132,7 @@
       <c r="C23" s="46">
         <v>40</v>
       </c>
-      <c r="D23" s="78">
+      <c r="D23" s="69">
         <v>2.2499999999999998E-3</v>
       </c>
     </row>
@@ -5143,7 +5143,7 @@
       <c r="C24" s="46">
         <v>50</v>
       </c>
-      <c r="D24" s="78">
+      <c r="D24" s="69">
         <v>2.0789999999999999E-2</v>
       </c>
     </row>
@@ -5154,7 +5154,7 @@
       <c r="C25" s="46">
         <v>60</v>
       </c>
-      <c r="D25" s="78">
+      <c r="D25" s="69">
         <v>4.3749999999999997E-2</v>
       </c>
     </row>
@@ -5165,7 +5165,7 @@
       <c r="C26" s="46">
         <v>70</v>
       </c>
-      <c r="D26" s="78">
+      <c r="D26" s="69">
         <v>8.2210000000000005E-2</v>
       </c>
     </row>
@@ -5176,53 +5176,53 @@
       <c r="C27" s="46">
         <v>80</v>
       </c>
-      <c r="D27" s="78">
+      <c r="D27" s="69">
         <v>0.14219000000000001</v>
       </c>
     </row>
     <row r="35" spans="6:12">
-      <c r="F35" s="78">
+      <c r="F35" s="69">
         <v>3.8999999999999999E-4</v>
       </c>
-      <c r="G35" s="78">
+      <c r="G35" s="69">
         <v>1.67E-3</v>
       </c>
-      <c r="H35" s="78">
+      <c r="H35" s="69">
         <v>4.64E-3</v>
       </c>
-      <c r="I35" s="78">
+      <c r="I35" s="69">
         <v>1.027E-2</v>
       </c>
-      <c r="J35" s="78">
+      <c r="J35" s="69">
         <v>1.966E-2</v>
       </c>
-      <c r="K35" s="78">
+      <c r="K35" s="69">
         <v>3.4029999999999998E-2</v>
       </c>
-      <c r="L35" s="78">
+      <c r="L35" s="69">
         <v>5.4739999999999997E-2</v>
       </c>
     </row>
     <row r="36" spans="6:12">
-      <c r="F36" s="78">
+      <c r="F36" s="69">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="G36" s="78">
+      <c r="G36" s="69">
         <v>5.5999999999999995E-4</v>
       </c>
-      <c r="H36" s="78">
+      <c r="H36" s="69">
         <v>2.2499999999999998E-3</v>
       </c>
-      <c r="I36" s="78">
+      <c r="I36" s="69">
         <v>2.0789999999999999E-2</v>
       </c>
-      <c r="J36" s="78">
+      <c r="J36" s="69">
         <v>4.3749999999999997E-2</v>
       </c>
-      <c r="K36" s="78">
+      <c r="K36" s="69">
         <v>8.2210000000000005E-2</v>
       </c>
-      <c r="L36" s="78">
+      <c r="L36" s="69">
         <v>0.14219000000000001</v>
       </c>
     </row>
@@ -6724,7 +6724,7 @@
         <v>6.88E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75">
+    <row r="14" spans="1:5">
       <c r="C14" t="s">
         <v>45</v>
       </c>
@@ -6859,7 +6859,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7069,7 +7069,7 @@
       <c r="D21">
         <v>20</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="70">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="F21" t="s">
@@ -7701,30 +7701,30 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
       <c r="C6" s="2"/>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72" t="s">
+      <c r="E6" s="73"/>
+      <c r="F6" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72" t="s">
+      <c r="G6" s="74"/>
+      <c r="H6" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="72"/>
-    </row>
-    <row r="7" spans="1:11" ht="25.5">
+      <c r="I6" s="74"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>

</xml_diff>